<commit_message>
downstream sorting - combining
</commit_message>
<xml_diff>
--- a/Figure Generating/data/DNA_Biofilm_Trans_Defense_Coverage.xlsx
+++ b/Figure Generating/data/DNA_Biofilm_Trans_Defense_Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin Juntao\Desktop\transposase-deep-ocean\Figure Generating\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A23974D-39DB-4C7B-B6A6-3F2A845E9201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D095AA-A7FF-405E-BD2D-5457D0AC1D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="624" windowWidth="21360" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
   <si>
     <t>TARA_X000000368</t>
   </si>
@@ -607,6 +607,12 @@
   </si>
   <si>
     <t>DNA_sect_CAZ</t>
+  </si>
+  <si>
+    <t>DNA_peptidase</t>
+  </si>
+  <si>
+    <t>DNA_sect_pep</t>
   </si>
 </sst>
 </file>
@@ -943,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K181"/>
+  <dimension ref="A1:M181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -962,7 +968,7 @@
     <col min="10" max="10" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6">
+    <row r="1" spans="1:13" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>180</v>
       </c>
@@ -996,8 +1002,14 @@
       <c r="K1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1034,8 +1046,14 @@
       <c r="K2">
         <v>2.56248619083885E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2">
+        <v>3.8437106589524601E-2</v>
+      </c>
+      <c r="M2">
+        <v>8.3316657947394099E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1072,8 +1090,14 @@
       <c r="K3">
         <v>3.0925117314035099E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3">
+        <v>4.0307176274845799E-2</v>
+      </c>
+      <c r="M3">
+        <v>8.9464381510720205E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1110,8 +1134,14 @@
       <c r="K4">
         <v>3.5566305304910902E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <v>3.86280959751455E-2</v>
+      </c>
+      <c r="M4">
+        <v>1.0161982549717801E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1148,8 +1178,14 @@
       <c r="K5">
         <v>1.02553535976059E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <v>2.6856325675505499E-2</v>
+      </c>
+      <c r="M5">
+        <v>4.07066236722416E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1186,8 +1222,14 @@
       <c r="K6">
         <v>1.9243435677656199E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <v>3.5460707952912701E-2</v>
+      </c>
+      <c r="M6">
+        <v>7.6395393154068403E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1224,8 +1266,14 @@
       <c r="K7">
         <v>1.8007842340642399E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <v>3.5669821242514499E-2</v>
+      </c>
+      <c r="M7">
+        <v>7.0503647795832399E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1262,8 +1310,14 @@
       <c r="K8">
         <v>1.25191593521696E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <v>3.0258444295056801E-2</v>
+      </c>
+      <c r="M8">
+        <v>4.71794941396971E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1300,8 +1354,14 @@
       <c r="K9">
         <v>3.6430158070262699E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9">
+        <v>4.6222620717537799E-2</v>
+      </c>
+      <c r="M9">
+        <v>1.1863482705294401E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1338,8 +1398,14 @@
       <c r="K10">
         <v>3.5454411649244802E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10">
+        <v>3.6934049757349499E-2</v>
+      </c>
+      <c r="M10">
+        <v>8.9132156380819592E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1376,8 +1442,14 @@
       <c r="K11">
         <v>1.95213978432168E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11">
+        <v>3.4733361694088798E-2</v>
+      </c>
+      <c r="M11">
+        <v>7.7387081043315499E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1414,8 +1486,14 @@
       <c r="K12">
         <v>2.27747601987096E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12">
+        <v>3.3956951796825799E-2</v>
+      </c>
+      <c r="M12">
+        <v>7.8670666006048495E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1452,8 +1530,14 @@
       <c r="K13">
         <v>1.9113280174829601E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13">
+        <v>2.7726508246430401E-2</v>
+      </c>
+      <c r="M13">
+        <v>6.5399039937055698E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1490,8 +1574,14 @@
       <c r="K14">
         <v>2.3558842537686601E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14">
+        <v>3.6335077104417898E-2</v>
+      </c>
+      <c r="M14">
+        <v>8.6882387340151603E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1528,8 +1618,14 @@
       <c r="K15">
         <v>2.3661793561490698E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15">
+        <v>3.6053147546787498E-2</v>
+      </c>
+      <c r="M15">
+        <v>8.7915765806195392E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1566,8 +1662,14 @@
       <c r="K16">
         <v>1.6900156538175301E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16">
+        <v>3.0597610695263198E-2</v>
+      </c>
+      <c r="M16">
+        <v>5.62977602469035E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1604,8 +1706,14 @@
       <c r="K17">
         <v>1.6592250857970399E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17">
+        <v>2.9842164582482001E-2</v>
+      </c>
+      <c r="M17">
+        <v>5.1658595473017604E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1642,8 +1750,14 @@
       <c r="K18">
         <v>1.9372748965632699E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18">
+        <v>3.1794812075955498E-2</v>
+      </c>
+      <c r="M18">
+        <v>6.1266955701898898E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1680,8 +1794,14 @@
       <c r="K19">
         <v>1.41646364555408E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19">
+        <v>2.9014651171705E-2</v>
+      </c>
+      <c r="M19">
+        <v>4.9387261221818099E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1718,8 +1838,14 @@
       <c r="K20">
         <v>1.6497364572940899E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20">
+        <v>3.3932220939926198E-2</v>
+      </c>
+      <c r="M20">
+        <v>6.3845509539485297E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1756,8 +1882,14 @@
       <c r="K21">
         <v>1.6180441515760099E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21">
+        <v>2.8095933368715201E-2</v>
+      </c>
+      <c r="M21">
+        <v>6.2543950155829397E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1794,8 +1926,14 @@
       <c r="K22">
         <v>1.7186838794445299E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22">
+        <v>3.02683440965681E-2</v>
+      </c>
+      <c r="M22">
+        <v>6.1384882361630397E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1832,8 +1970,14 @@
       <c r="K23">
         <v>1.57862964623772E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23">
+        <v>2.9744341077088201E-2</v>
+      </c>
+      <c r="M23">
+        <v>5.9243859739518999E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1870,8 +2014,14 @@
       <c r="K24">
         <v>1.4249006850150501E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24">
+        <v>2.5347500657914301E-2</v>
+      </c>
+      <c r="M24">
+        <v>4.3165348522356001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1908,8 +2058,14 @@
       <c r="K25">
         <v>1.33536532826741E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25">
+        <v>3.0159588081919701E-2</v>
+      </c>
+      <c r="M25">
+        <v>4.7917131072330102E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1946,8 +2102,14 @@
       <c r="K26">
         <v>1.2404072203839899E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26">
+        <v>3.0786830227507798E-2</v>
+      </c>
+      <c r="M26">
+        <v>6.0511584784876697E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1984,8 +2146,14 @@
       <c r="K27">
         <v>1.40724646034208E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27">
+        <v>3.1847934926133303E-2</v>
+      </c>
+      <c r="M27">
+        <v>4.9451015046818002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2022,8 +2190,14 @@
       <c r="K28">
         <v>1.68138290333803E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28">
+        <v>3.3978851293892699E-2</v>
+      </c>
+      <c r="M28">
+        <v>6.8458598250570497E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2060,8 +2234,14 @@
       <c r="K29">
         <v>1.38468068875193E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29">
+        <v>3.0853474418609601E-2</v>
+      </c>
+      <c r="M29">
+        <v>6.2598929847232504E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -2098,8 +2278,14 @@
       <c r="K30">
         <v>1.5175238350445201E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30">
+        <v>3.39216073244097E-2</v>
+      </c>
+      <c r="M30">
+        <v>5.4750877401099299E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2136,8 +2322,14 @@
       <c r="K31">
         <v>1.3409876962956499E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31">
+        <v>2.8496185124864501E-2</v>
+      </c>
+      <c r="M31">
+        <v>4.3465749319269702E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2174,8 +2366,14 @@
       <c r="K32">
         <v>1.4167249987181499E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32">
+        <v>2.95478537427563E-2</v>
+      </c>
+      <c r="M32">
+        <v>6.3119318926649296E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2212,8 +2410,14 @@
       <c r="K33">
         <v>2.74523745133722E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33">
+        <v>4.1764251299440502E-2</v>
+      </c>
+      <c r="M33">
+        <v>1.5555316589937701E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2250,8 +2454,14 @@
       <c r="K34">
         <v>4.2972817950856701E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34">
+        <v>3.2158222500444797E-2</v>
+      </c>
+      <c r="M34">
+        <v>1.04419415935627E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2288,8 +2498,14 @@
       <c r="K35">
         <v>1.75572519548022E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35">
+        <v>3.3908428310322203E-2</v>
+      </c>
+      <c r="M35">
+        <v>6.6774787097068104E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2326,8 +2542,14 @@
       <c r="K36">
         <v>1.8798553581876899E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36">
+        <v>2.9469783222085801E-2</v>
+      </c>
+      <c r="M36">
+        <v>6.3047809094146099E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2364,8 +2586,14 @@
       <c r="K37">
         <v>1.7955699080202999E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37">
+        <v>2.84160746165028E-2</v>
+      </c>
+      <c r="M37">
+        <v>6.3141709139210699E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -2402,8 +2630,14 @@
       <c r="K38">
         <v>1.0790773736108199E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38">
+        <v>1.96231794457381E-2</v>
+      </c>
+      <c r="M38">
+        <v>3.5195232485872099E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2440,8 +2674,14 @@
       <c r="K39">
         <v>1.9345877595192201E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39">
+        <v>2.9540786334944599E-2</v>
+      </c>
+      <c r="M39">
+        <v>7.03479020745576E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -2478,8 +2718,14 @@
       <c r="K40">
         <v>4.6287374670973798E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40">
+        <v>3.7065001413193098E-2</v>
+      </c>
+      <c r="M40">
+        <v>1.2473746440413901E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2516,8 +2762,14 @@
       <c r="K41">
         <v>1.3904960718775501E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41">
+        <v>1.83054814645702E-2</v>
+      </c>
+      <c r="M41">
+        <v>4.37609649340786E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2554,8 +2806,14 @@
       <c r="K42">
         <v>1.7496197861422401E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42">
+        <v>2.98627774941643E-2</v>
+      </c>
+      <c r="M42">
+        <v>6.5272575138982797E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2592,8 +2850,14 @@
       <c r="K43">
         <v>2.1236754955568102E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43">
+        <v>2.8685633982918599E-2</v>
+      </c>
+      <c r="M43">
+        <v>6.1776161216754999E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2630,8 +2894,14 @@
       <c r="K44">
         <v>2.0464311437013898E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44">
+        <v>2.89751438505873E-2</v>
+      </c>
+      <c r="M44">
+        <v>6.2910285928486197E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2668,8 +2938,14 @@
       <c r="K45">
         <v>2.2346344298592E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45">
+        <v>2.83992838671039E-2</v>
+      </c>
+      <c r="M45">
+        <v>6.8383826447054501E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -2706,8 +2982,14 @@
       <c r="K46">
         <v>2.0114509553836799E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46">
+        <v>2.6024908790981301E-2</v>
+      </c>
+      <c r="M46">
+        <v>6.38954000284697E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2744,8 +3026,14 @@
       <c r="K47">
         <v>8.6683794872662804E-4</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47">
+        <v>1.6144798350799301E-2</v>
+      </c>
+      <c r="M47">
+        <v>3.0665442025675999E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -2782,8 +3070,14 @@
       <c r="K48">
         <v>1.824473229162E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48">
+        <v>1.78521622338264E-2</v>
+      </c>
+      <c r="M48">
+        <v>4.6163597861979301E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2820,8 +3114,14 @@
       <c r="K49">
         <v>1.2798722421446401E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49">
+        <v>2.4629207219047499E-2</v>
+      </c>
+      <c r="M49">
+        <v>4.1314424134086397E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2858,8 +3158,14 @@
       <c r="K50">
         <v>1.9774008415486899E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50">
+        <v>2.7933876920376199E-2</v>
+      </c>
+      <c r="M50">
+        <v>5.8690046088717297E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>92</v>
       </c>
@@ -2896,8 +3202,14 @@
       <c r="K51">
         <v>2.2577560325177E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51">
+        <v>3.3486785841008997E-2</v>
+      </c>
+      <c r="M51">
+        <v>8.1393425725092595E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>90</v>
       </c>
@@ -2934,8 +3246,14 @@
       <c r="K52">
         <v>1.9729972329236602E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52">
+        <v>3.3537190199578903E-2</v>
+      </c>
+      <c r="M52">
+        <v>7.7256792874708302E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>91</v>
       </c>
@@ -2972,8 +3290,14 @@
       <c r="K53">
         <v>1.9101191092301001E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53">
+        <v>3.2066030630954402E-2</v>
+      </c>
+      <c r="M53">
+        <v>7.5502597619708E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -3010,8 +3334,14 @@
       <c r="K54">
         <v>2.9793278152848799E-3</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54">
+        <v>3.5544252718790803E-2</v>
+      </c>
+      <c r="M54">
+        <v>9.6844326430508398E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -3048,8 +3378,14 @@
       <c r="K55">
         <v>3.04300884825307E-3</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55">
+        <v>3.4342369352365398E-2</v>
+      </c>
+      <c r="M55">
+        <v>9.4744513388875899E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -3086,8 +3422,14 @@
       <c r="K56">
         <v>2.7148706230627801E-3</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56">
+        <v>3.6722480181342998E-2</v>
+      </c>
+      <c r="M56">
+        <v>9.1698474937302096E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -3124,8 +3466,14 @@
       <c r="K57">
         <v>3.1188158558069601E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="L57">
+        <v>4.0600503761446798E-2</v>
+      </c>
+      <c r="M57">
+        <v>9.9481730043812708E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -3162,8 +3510,14 @@
       <c r="K58">
         <v>2.4451080222918299E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="L58">
+        <v>3.2002647212152097E-2</v>
+      </c>
+      <c r="M58">
+        <v>8.3014119167995008E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>100</v>
       </c>
@@ -3200,8 +3554,14 @@
       <c r="K59">
         <v>2.9920474743505999E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="L59">
+        <v>2.9240910768473599E-2</v>
+      </c>
+      <c r="M59">
+        <v>7.9534159555262902E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>99</v>
       </c>
@@ -3238,8 +3598,14 @@
       <c r="K60">
         <v>2.1153899045647201E-3</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="L60">
+        <v>3.3728807972256102E-2</v>
+      </c>
+      <c r="M60">
+        <v>7.7262607697775997E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -3276,8 +3642,14 @@
       <c r="K61">
         <v>2.8510012278652498E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="L61">
+        <v>3.4407030557890399E-2</v>
+      </c>
+      <c r="M61">
+        <v>9.2137205279519806E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -3314,8 +3686,14 @@
       <c r="K62">
         <v>1.24558950279848E-3</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="L62">
+        <v>2.5728734074101301E-2</v>
+      </c>
+      <c r="M62">
+        <v>4.5717760884355198E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -3352,8 +3730,14 @@
       <c r="K63">
         <v>1.6410259170465901E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63">
+        <v>2.63079551347059E-2</v>
+      </c>
+      <c r="M63">
+        <v>5.6204617452887996E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -3390,8 +3774,14 @@
       <c r="K64">
         <v>3.3041094632767802E-3</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="L64">
+        <v>3.7673123570132298E-2</v>
+      </c>
+      <c r="M64">
+        <v>1.15313739044997E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -3428,8 +3818,14 @@
       <c r="K65">
         <v>3.1719483235937598E-3</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="L65">
+        <v>3.3698567403086799E-2</v>
+      </c>
+      <c r="M65">
+        <v>1.06631082392396E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -3466,8 +3862,14 @@
       <c r="K66">
         <v>2.4088111155165198E-3</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="L66">
+        <v>3.0297047288060701E-2</v>
+      </c>
+      <c r="M66">
+        <v>9.4932282950734095E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -3504,8 +3906,14 @@
       <c r="K67">
         <v>2.6542955167628401E-3</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67">
+        <v>3.51094099195218E-2</v>
+      </c>
+      <c r="M67">
+        <v>1.15643587700973E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -3542,8 +3950,14 @@
       <c r="K68">
         <v>2.1405706438753298E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="L68">
+        <v>2.9397914443190801E-2</v>
+      </c>
+      <c r="M68">
+        <v>8.7580355274833894E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -3580,8 +3994,14 @@
       <c r="K69">
         <v>2.1081768731753899E-3</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="L69">
+        <v>2.8063991257634899E-2</v>
+      </c>
+      <c r="M69">
+        <v>7.1377456463740802E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -3618,8 +4038,14 @@
       <c r="K70">
         <v>1.87205750486137E-3</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="L70">
+        <v>2.99660518447958E-2</v>
+      </c>
+      <c r="M70">
+        <v>5.690381320548E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -3656,8 +4082,14 @@
       <c r="K71">
         <v>2.4344223769726101E-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="L71">
+        <v>3.2654823496197798E-2</v>
+      </c>
+      <c r="M71">
+        <v>7.7993521248993902E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -3694,8 +4126,14 @@
       <c r="K72">
         <v>1.86325824592621E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72">
+        <v>2.9021987484911499E-2</v>
+      </c>
+      <c r="M72">
+        <v>6.2870650660376099E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -3732,8 +4170,14 @@
       <c r="K73">
         <v>3.0674987099628898E-3</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="L73">
+        <v>3.6128081521538999E-2</v>
+      </c>
+      <c r="M73">
+        <v>8.4433694045829392E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -3770,8 +4214,14 @@
       <c r="K74">
         <v>2.7678828122651598E-3</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="L74">
+        <v>3.2652523146291301E-2</v>
+      </c>
+      <c r="M74">
+        <v>7.72936931676051E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -3808,8 +4258,14 @@
       <c r="K75">
         <v>2.7187748367629499E-3</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="L75">
+        <v>3.2558768474367901E-2</v>
+      </c>
+      <c r="M75">
+        <v>8.8810103066433391E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
       <c r="A76" t="s">
         <v>95</v>
       </c>
@@ -3846,8 +4302,14 @@
       <c r="K76">
         <v>1.79728790987948E-3</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="L76">
+        <v>2.62980716899151E-2</v>
+      </c>
+      <c r="M76">
+        <v>5.0416144563517999E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>93</v>
       </c>
@@ -3884,8 +4346,14 @@
       <c r="K77">
         <v>1.8393437699944701E-3</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77">
+        <v>2.5900104444965499E-2</v>
+      </c>
+      <c r="M77">
+        <v>6.0274657987651201E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>94</v>
       </c>
@@ -3922,8 +4390,14 @@
       <c r="K78">
         <v>4.0222618685700502E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="L78">
+        <v>3.2985515236838403E-2</v>
+      </c>
+      <c r="M78">
+        <v>9.8310990853929595E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -3960,8 +4434,14 @@
       <c r="K79">
         <v>2.2977680110193399E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="L79">
+        <v>3.3322855876399902E-2</v>
+      </c>
+      <c r="M79">
+        <v>8.0297448847907894E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -3998,8 +4478,14 @@
       <c r="K80">
         <v>3.11318250584359E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="L80">
+        <v>3.9632229881838801E-2</v>
+      </c>
+      <c r="M80">
+        <v>1.0543374555236599E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -4036,8 +4522,14 @@
       <c r="K81">
         <v>3.7680696234718199E-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="L81">
+        <v>3.9731778149778102E-2</v>
+      </c>
+      <c r="M81">
+        <v>1.0928790470282701E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -4074,8 +4566,14 @@
       <c r="K82">
         <v>2.6636871874945599E-3</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="L82">
+        <v>3.4948672703872301E-2</v>
+      </c>
+      <c r="M82">
+        <v>9.2059805304147008E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
       <c r="A83" t="s">
         <v>73</v>
       </c>
@@ -4112,8 +4610,14 @@
       <c r="K83">
         <v>2.1724133749920602E-3</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="L83">
+        <v>3.2443248233743803E-2</v>
+      </c>
+      <c r="M83">
+        <v>6.2231129180221499E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" t="s">
         <v>75</v>
       </c>
@@ -4150,8 +4654,14 @@
       <c r="K84">
         <v>1.2395284579149999E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84">
+        <v>2.7050986337532501E-2</v>
+      </c>
+      <c r="M84">
+        <v>5.4385227612507303E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" t="s">
         <v>76</v>
       </c>
@@ -4188,8 +4698,14 @@
       <c r="K85">
         <v>1.69293896115063E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="L85">
+        <v>2.75917966340926E-2</v>
+      </c>
+      <c r="M85">
+        <v>5.04918426137163E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -4226,8 +4742,14 @@
       <c r="K86">
         <v>1.67373669353275E-3</v>
       </c>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="L86">
+        <v>2.7862350194692E-2</v>
+      </c>
+      <c r="M86">
+        <v>5.7148754998064301E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" t="s">
         <v>72</v>
       </c>
@@ -4264,8 +4786,14 @@
       <c r="K87">
         <v>3.2496648334157702E-3</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
+      <c r="L87">
+        <v>3.9515202561713203E-2</v>
+      </c>
+      <c r="M87">
+        <v>8.7894288386736602E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
       <c r="A88" t="s">
         <v>70</v>
       </c>
@@ -4302,8 +4830,14 @@
       <c r="K88">
         <v>5.2674177969941503E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:11">
+      <c r="L88">
+        <v>4.4042614066619898E-2</v>
+      </c>
+      <c r="M88">
+        <v>1.47702920729193E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" t="s">
         <v>71</v>
       </c>
@@ -4340,8 +4874,14 @@
       <c r="K89">
         <v>4.0055200060356297E-3</v>
       </c>
-    </row>
-    <row r="90" spans="1:11">
+      <c r="L89">
+        <v>3.7916221935526899E-2</v>
+      </c>
+      <c r="M89">
+        <v>1.10533080385079E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -4378,8 +4918,14 @@
       <c r="K90">
         <v>2.2075778027744E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
+      <c r="L90">
+        <v>3.2391900907091403E-2</v>
+      </c>
+      <c r="M90">
+        <v>7.93242884639077E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" t="s">
         <v>112</v>
       </c>
@@ -4416,8 +4962,14 @@
       <c r="K91">
         <v>2.99184032070955E-3</v>
       </c>
-    </row>
-    <row r="92" spans="1:11">
+      <c r="L91">
+        <v>3.3516245707581403E-2</v>
+      </c>
+      <c r="M91">
+        <v>7.3728334303028199E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" t="s">
         <v>110</v>
       </c>
@@ -4454,8 +5006,14 @@
       <c r="K92">
         <v>1.9662586781774602E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="L92">
+        <v>2.8555125635174899E-2</v>
+      </c>
+      <c r="M92">
+        <v>6.2935431595858302E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" t="s">
         <v>111</v>
       </c>
@@ -4492,8 +5050,14 @@
       <c r="K93">
         <v>1.75427808663334E-3</v>
       </c>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="L93">
+        <v>3.0157076081159299E-2</v>
+      </c>
+      <c r="M93">
+        <v>6.6194841726207702E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" t="s">
         <v>89</v>
       </c>
@@ -4530,8 +5094,14 @@
       <c r="K94">
         <v>2.5903829962155502E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="L94">
+        <v>3.5533759628648201E-2</v>
+      </c>
+      <c r="M94">
+        <v>8.7542524887552504E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -4568,8 +5138,14 @@
       <c r="K95">
         <v>2.5573272009614301E-3</v>
       </c>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="L95">
+        <v>3.4987440477042199E-2</v>
+      </c>
+      <c r="M95">
+        <v>9.2661777797429599E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -4606,8 +5182,14 @@
       <c r="K96">
         <v>2.5917971974469501E-3</v>
       </c>
-    </row>
-    <row r="97" spans="1:11">
+      <c r="L96">
+        <v>3.6594592755358202E-2</v>
+      </c>
+      <c r="M96">
+        <v>9.4499788481472499E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -4644,8 +5226,14 @@
       <c r="K97">
         <v>2.4572214247651201E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:11">
+      <c r="L97">
+        <v>3.8836136600336302E-2</v>
+      </c>
+      <c r="M97">
+        <v>9.6080612304736603E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -4682,8 +5270,14 @@
       <c r="K98">
         <v>2.9455665199934599E-3</v>
       </c>
-    </row>
-    <row r="99" spans="1:11">
+      <c r="L98">
+        <v>3.5057462129368701E-2</v>
+      </c>
+      <c r="M98">
+        <v>8.7376318644580894E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" t="s">
         <v>125</v>
       </c>
@@ -4720,8 +5314,14 @@
       <c r="K99">
         <v>2.0477530455583698E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="L99">
+        <v>3.2571601561914403E-2</v>
+      </c>
+      <c r="M99">
+        <v>7.8134526607806093E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" t="s">
         <v>124</v>
       </c>
@@ -4758,8 +5358,14 @@
       <c r="K100">
         <v>2.32879046968873E-3</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="L100">
+        <v>3.1280241100798703E-2</v>
+      </c>
+      <c r="M100">
+        <v>7.6834950778595099E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
       <c r="A101" t="s">
         <v>126</v>
       </c>
@@ -4796,8 +5402,14 @@
       <c r="K101">
         <v>1.6526764994326301E-3</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="L101">
+        <v>2.6372683872885199E-2</v>
+      </c>
+      <c r="M101">
+        <v>5.7939299953876297E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
       <c r="A102" t="s">
         <v>138</v>
       </c>
@@ -4834,8 +5446,14 @@
       <c r="K102">
         <v>2.7524582275087299E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:11">
+      <c r="L102">
+        <v>3.54828569946984E-2</v>
+      </c>
+      <c r="M102">
+        <v>8.9240155548230907E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
       <c r="A103" t="s">
         <v>137</v>
       </c>
@@ -4872,8 +5490,14 @@
       <c r="K103">
         <v>2.5905378776206502E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="L103">
+        <v>3.3339381210791497E-2</v>
+      </c>
+      <c r="M103">
+        <v>8.49814798105877E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
       <c r="A104" t="s">
         <v>136</v>
       </c>
@@ -4910,8 +5534,14 @@
       <c r="K104">
         <v>1.75801375154807E-3</v>
       </c>
-    </row>
-    <row r="105" spans="1:11">
+      <c r="L104">
+        <v>2.8661045547340801E-2</v>
+      </c>
+      <c r="M104">
+        <v>6.4776982983443601E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -4948,8 +5578,14 @@
       <c r="K105">
         <v>1.89641821197057E-3</v>
       </c>
-    </row>
-    <row r="106" spans="1:11">
+      <c r="L105">
+        <v>2.8743885133800402E-2</v>
+      </c>
+      <c r="M105">
+        <v>6.7519622006340903E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
       <c r="A106" t="s">
         <v>109</v>
       </c>
@@ -4986,8 +5622,14 @@
       <c r="K106">
         <v>1.65285372358029E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:11">
+      <c r="L106">
+        <v>2.99012106987964E-2</v>
+      </c>
+      <c r="M106">
+        <v>5.4266757521490199E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -5024,8 +5666,14 @@
       <c r="K107">
         <v>1.3817106298537199E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="L107">
+        <v>2.60428159030466E-2</v>
+      </c>
+      <c r="M107">
+        <v>6.2490201153130899E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -5062,8 +5710,14 @@
       <c r="K108">
         <v>2.23599729905157E-3</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="L108">
+        <v>3.5130273590420799E-2</v>
+      </c>
+      <c r="M108">
+        <v>7.72243343557157E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13">
       <c r="A109" t="s">
         <v>127</v>
       </c>
@@ -5100,8 +5754,14 @@
       <c r="K109">
         <v>2.38651521818574E-3</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="L109">
+        <v>3.5769852748161197E-2</v>
+      </c>
+      <c r="M109">
+        <v>8.3937893912190698E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13">
       <c r="A110" t="s">
         <v>134</v>
       </c>
@@ -5138,8 +5798,14 @@
       <c r="K110">
         <v>2.6200634849442598E-3</v>
       </c>
-    </row>
-    <row r="111" spans="1:11">
+      <c r="L110">
+        <v>3.3782610376235103E-2</v>
+      </c>
+      <c r="M110">
+        <v>7.9944875906187395E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
       <c r="A111" t="s">
         <v>135</v>
       </c>
@@ -5176,8 +5842,14 @@
       <c r="K111">
         <v>2.6223649302711699E-3</v>
       </c>
-    </row>
-    <row r="112" spans="1:11">
+      <c r="L111">
+        <v>3.4982283913107003E-2</v>
+      </c>
+      <c r="M111">
+        <v>8.1164814078730305E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -5214,8 +5886,14 @@
       <c r="K112">
         <v>2.36562535943589E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
+      <c r="L112">
+        <v>3.4845971724736101E-2</v>
+      </c>
+      <c r="M112">
+        <v>8.1101962815039296E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -5252,8 +5930,14 @@
       <c r="K113">
         <v>1.7583739976820599E-3</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
+      <c r="L113">
+        <v>2.8774234398431402E-2</v>
+      </c>
+      <c r="M113">
+        <v>6.9821857177816398E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13">
       <c r="A114" t="s">
         <v>131</v>
       </c>
@@ -5290,8 +5974,14 @@
       <c r="K114">
         <v>2.1680377933031999E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
+      <c r="L114">
+        <v>3.3824695972597803E-2</v>
+      </c>
+      <c r="M114">
+        <v>8.2670858997872295E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -5328,8 +6018,14 @@
       <c r="K115">
         <v>1.7436866310001999E-3</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="L115">
+        <v>2.7262327495110199E-2</v>
+      </c>
+      <c r="M115">
+        <v>6.0285061309382501E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13">
       <c r="A116" t="s">
         <v>133</v>
       </c>
@@ -5366,8 +6062,14 @@
       <c r="K116">
         <v>2.3649848265379801E-3</v>
       </c>
-    </row>
-    <row r="117" spans="1:11">
+      <c r="L116">
+        <v>3.3185983137452801E-2</v>
+      </c>
+      <c r="M116">
+        <v>7.3044518391520499E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -5404,8 +6106,14 @@
       <c r="K117">
         <v>2.7521925425754499E-3</v>
       </c>
-    </row>
-    <row r="118" spans="1:11">
+      <c r="L117">
+        <v>3.3640364139289398E-2</v>
+      </c>
+      <c r="M117">
+        <v>8.2221451451985495E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13">
       <c r="A118" t="s">
         <v>120</v>
       </c>
@@ -5442,8 +6150,14 @@
       <c r="K118">
         <v>2.3176926316110301E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:11">
+      <c r="L118">
+        <v>3.2507261823641498E-2</v>
+      </c>
+      <c r="M118">
+        <v>6.9212937627117204E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
       <c r="A119" t="s">
         <v>113</v>
       </c>
@@ -5480,8 +6194,14 @@
       <c r="K119">
         <v>2.6583133928241198E-3</v>
       </c>
-    </row>
-    <row r="120" spans="1:11">
+      <c r="L119">
+        <v>3.8478598242308398E-2</v>
+      </c>
+      <c r="M119">
+        <v>1.05709167174971E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13">
       <c r="A120" t="s">
         <v>114</v>
       </c>
@@ -5518,8 +6238,14 @@
       <c r="K120">
         <v>2.91038535586804E-3</v>
       </c>
-    </row>
-    <row r="121" spans="1:11">
+      <c r="L120">
+        <v>3.6915111617383603E-2</v>
+      </c>
+      <c r="M120">
+        <v>1.12613861580386E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -5556,8 +6282,14 @@
       <c r="K121">
         <v>1.6333485041133799E-3</v>
       </c>
-    </row>
-    <row r="122" spans="1:11">
+      <c r="L121">
+        <v>2.8588810338575299E-2</v>
+      </c>
+      <c r="M121">
+        <v>5.2667692066990001E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13">
       <c r="A122" t="s">
         <v>116</v>
       </c>
@@ -5594,8 +6326,14 @@
       <c r="K122">
         <v>1.1520584936853301E-3</v>
       </c>
-    </row>
-    <row r="123" spans="1:11">
+      <c r="L122">
+        <v>2.5553936878511999E-2</v>
+      </c>
+      <c r="M122">
+        <v>5.2280091339347501E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13">
       <c r="A123" t="s">
         <v>117</v>
       </c>
@@ -5632,8 +6370,14 @@
       <c r="K123">
         <v>2.9222469758202999E-3</v>
       </c>
-    </row>
-    <row r="124" spans="1:11">
+      <c r="L123">
+        <v>3.5437162877555897E-2</v>
+      </c>
+      <c r="M123">
+        <v>1.09402223908653E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13">
       <c r="A124" t="s">
         <v>119</v>
       </c>
@@ -5670,8 +6414,14 @@
       <c r="K124">
         <v>2.0047612890418702E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:11">
+      <c r="L124">
+        <v>3.1564738059720099E-2</v>
+      </c>
+      <c r="M124">
+        <v>6.2384549139398501E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -5708,8 +6458,14 @@
       <c r="K125">
         <v>3.52388931384755E-3</v>
       </c>
-    </row>
-    <row r="126" spans="1:11">
+      <c r="L125">
+        <v>3.3153262394410903E-2</v>
+      </c>
+      <c r="M125">
+        <v>9.8227395934595493E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -5746,8 +6502,14 @@
       <c r="K126">
         <v>2.17055161661488E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:11">
+      <c r="L126">
+        <v>3.7145777713616997E-2</v>
+      </c>
+      <c r="M126">
+        <v>8.8720614402111805E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
       <c r="A127" t="s">
         <v>121</v>
       </c>
@@ -5784,8 +6546,14 @@
       <c r="K127">
         <v>2.5312317376415699E-3</v>
       </c>
-    </row>
-    <row r="128" spans="1:11">
+      <c r="L127">
+        <v>3.7665839747317E-2</v>
+      </c>
+      <c r="M127">
+        <v>9.5260431809676901E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
       <c r="A128" t="s">
         <v>141</v>
       </c>
@@ -5822,8 +6590,14 @@
       <c r="K128">
         <v>4.0669978062649404E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:11">
+      <c r="L128">
+        <v>4.2586291150179402E-2</v>
+      </c>
+      <c r="M128">
+        <v>1.19353957522672E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13">
       <c r="A129" t="s">
         <v>139</v>
       </c>
@@ -5860,8 +6634,14 @@
       <c r="K129">
         <v>2.9121999200374601E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:11">
+      <c r="L129">
+        <v>3.9695847709189797E-2</v>
+      </c>
+      <c r="M129">
+        <v>1.02000156358112E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13">
       <c r="A130" t="s">
         <v>140</v>
       </c>
@@ -5898,8 +6678,14 @@
       <c r="K130">
         <v>1.61825797164784E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:11">
+      <c r="L130">
+        <v>3.0341447375166E-2</v>
+      </c>
+      <c r="M130">
+        <v>6.8603038803077996E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
       <c r="A131" t="s">
         <v>149</v>
       </c>
@@ -5936,8 +6722,14 @@
       <c r="K131">
         <v>5.53895919772568E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:11">
+      <c r="L131">
+        <v>4.0253422774438399E-2</v>
+      </c>
+      <c r="M131">
+        <v>1.4598654292125699E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13">
       <c r="A132" t="s">
         <v>148</v>
       </c>
@@ -5974,8 +6766,14 @@
       <c r="K132">
         <v>5.2874066207456404E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:11">
+      <c r="L132">
+        <v>4.0943635040340397E-2</v>
+      </c>
+      <c r="M132">
+        <v>1.39807558038716E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -6012,8 +6810,14 @@
       <c r="K133">
         <v>5.0333721571194099E-3</v>
       </c>
-    </row>
-    <row r="134" spans="1:11">
+      <c r="L133">
+        <v>3.7931089665537703E-2</v>
+      </c>
+      <c r="M133">
+        <v>1.39885037765143E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13">
       <c r="A134" t="s">
         <v>152</v>
       </c>
@@ -6050,8 +6854,14 @@
       <c r="K134">
         <v>5.2099871422946198E-3</v>
       </c>
-    </row>
-    <row r="135" spans="1:11">
+      <c r="L134">
+        <v>4.9260780154097399E-2</v>
+      </c>
+      <c r="M134">
+        <v>1.82387020375008E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13">
       <c r="A135" t="s">
         <v>151</v>
       </c>
@@ -6088,8 +6898,14 @@
       <c r="K135">
         <v>4.9186469384726803E-3</v>
       </c>
-    </row>
-    <row r="136" spans="1:11">
+      <c r="L135">
+        <v>4.8353756337092997E-2</v>
+      </c>
+      <c r="M135">
+        <v>1.7327482697513601E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -6126,8 +6942,14 @@
       <c r="K136">
         <v>4.7794397411544997E-3</v>
       </c>
-    </row>
-    <row r="137" spans="1:11">
+      <c r="L136">
+        <v>4.5575213742406202E-2</v>
+      </c>
+      <c r="M136">
+        <v>1.65237161682181E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13">
       <c r="A137" t="s">
         <v>153</v>
       </c>
@@ -6164,8 +6986,14 @@
       <c r="K137">
         <v>6.3605602620288304E-3</v>
       </c>
-    </row>
-    <row r="138" spans="1:11">
+      <c r="L137">
+        <v>5.2466800898783701E-2</v>
+      </c>
+      <c r="M137">
+        <v>2.0650132599920198E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13">
       <c r="A138" t="s">
         <v>154</v>
       </c>
@@ -6202,8 +7030,14 @@
       <c r="K138">
         <v>2.7206011012123402E-3</v>
       </c>
-    </row>
-    <row r="139" spans="1:11">
+      <c r="L138">
+        <v>3.6102929913419603E-2</v>
+      </c>
+      <c r="M138">
+        <v>9.6970194850892998E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -6240,8 +7074,14 @@
       <c r="K139">
         <v>2.03001075895021E-3</v>
       </c>
-    </row>
-    <row r="140" spans="1:11">
+      <c r="L139">
+        <v>2.9547456709924001E-2</v>
+      </c>
+      <c r="M139">
+        <v>7.4568448404734302E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13">
       <c r="A140" t="s">
         <v>155</v>
       </c>
@@ -6278,8 +7118,14 @@
       <c r="K140">
         <v>4.6887851221545998E-3</v>
       </c>
-    </row>
-    <row r="141" spans="1:11">
+      <c r="L140">
+        <v>4.0465235478028001E-2</v>
+      </c>
+      <c r="M140">
+        <v>1.40341191162254E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13">
       <c r="A141" t="s">
         <v>157</v>
       </c>
@@ -6316,8 +7162,14 @@
       <c r="K141">
         <v>4.5572913396745096E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:11">
+      <c r="L141">
+        <v>4.1862867656919898E-2</v>
+      </c>
+      <c r="M141">
+        <v>1.5664474110533198E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13">
       <c r="A142" t="s">
         <v>159</v>
       </c>
@@ -6354,8 +7206,14 @@
       <c r="K142">
         <v>4.5874031917162604E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:11">
+      <c r="L142">
+        <v>4.4777482052587601E-2</v>
+      </c>
+      <c r="M142">
+        <v>1.52325524023231E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13">
       <c r="A143" t="s">
         <v>158</v>
       </c>
@@ -6392,8 +7250,14 @@
       <c r="K143">
         <v>4.2366899338641502E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:11">
+      <c r="L143">
+        <v>4.3148770331021803E-2</v>
+      </c>
+      <c r="M143">
+        <v>1.4166716430653099E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13">
       <c r="A144" t="s">
         <v>162</v>
       </c>
@@ -6430,8 +7294,14 @@
       <c r="K144">
         <v>4.4067645829504497E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:11">
+      <c r="L144">
+        <v>4.2807662103137502E-2</v>
+      </c>
+      <c r="M144">
+        <v>1.47733623732949E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13">
       <c r="A145" t="s">
         <v>160</v>
       </c>
@@ -6468,8 +7338,14 @@
       <c r="K145">
         <v>3.5803999828298398E-3</v>
       </c>
-    </row>
-    <row r="146" spans="1:11">
+      <c r="L145">
+        <v>3.7489324747111502E-2</v>
+      </c>
+      <c r="M145">
+        <v>1.1739645819578299E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -6506,8 +7382,14 @@
       <c r="K146">
         <v>2.14824235863948E-3</v>
       </c>
-    </row>
-    <row r="147" spans="1:11">
+      <c r="L146">
+        <v>3.3592774833807397E-2</v>
+      </c>
+      <c r="M146">
+        <v>8.0662636031163405E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13">
       <c r="A147" t="s">
         <v>163</v>
       </c>
@@ -6544,8 +7426,14 @@
       <c r="K147">
         <v>2.3664665125553799E-3</v>
       </c>
-    </row>
-    <row r="148" spans="1:11">
+      <c r="L147">
+        <v>2.2651684140328299E-2</v>
+      </c>
+      <c r="M147">
+        <v>7.0679903360454203E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13">
       <c r="A148" t="s">
         <v>167</v>
       </c>
@@ -6582,8 +7470,14 @@
       <c r="K148">
         <v>4.0759888256797598E-3</v>
       </c>
-    </row>
-    <row r="149" spans="1:11">
+      <c r="L148">
+        <v>3.6518393296612398E-2</v>
+      </c>
+      <c r="M148">
+        <v>1.1520382948812E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13">
       <c r="A149" t="s">
         <v>178</v>
       </c>
@@ -6620,8 +7514,14 @@
       <c r="K149">
         <v>2.3179829018212298E-3</v>
       </c>
-    </row>
-    <row r="150" spans="1:11">
+      <c r="L149">
+        <v>3.23301988759081E-2</v>
+      </c>
+      <c r="M149">
+        <v>7.98711492557104E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13">
       <c r="A150" t="s">
         <v>179</v>
       </c>
@@ -6658,8 +7558,14 @@
       <c r="K150">
         <v>2.7084811618199702E-3</v>
       </c>
-    </row>
-    <row r="151" spans="1:11">
+      <c r="L150">
+        <v>3.5973173016671599E-2</v>
+      </c>
+      <c r="M150">
+        <v>9.9012503723037194E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13">
       <c r="A151" t="s">
         <v>177</v>
       </c>
@@ -6696,8 +7602,14 @@
       <c r="K151">
         <v>3.99878327981717E-3</v>
       </c>
-    </row>
-    <row r="152" spans="1:11">
+      <c r="L151">
+        <v>4.0793548906474797E-2</v>
+      </c>
+      <c r="M151">
+        <v>1.3448895938685E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13">
       <c r="A152" t="s">
         <v>176</v>
       </c>
@@ -6734,8 +7646,14 @@
       <c r="K152">
         <v>2.4888048947511901E-3</v>
       </c>
-    </row>
-    <row r="153" spans="1:11">
+      <c r="L152">
+        <v>3.11155907835362E-2</v>
+      </c>
+      <c r="M152">
+        <v>7.8343306649127607E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13">
       <c r="A153" t="s">
         <v>174</v>
       </c>
@@ -6772,8 +7690,14 @@
       <c r="K153">
         <v>3.85412676216216E-3</v>
       </c>
-    </row>
-    <row r="154" spans="1:11">
+      <c r="L153">
+        <v>3.5894951019381602E-2</v>
+      </c>
+      <c r="M153">
+        <v>1.10635147216706E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13">
       <c r="A154" t="s">
         <v>173</v>
       </c>
@@ -6810,8 +7734,14 @@
       <c r="K154">
         <v>2.5075288145543499E-3</v>
       </c>
-    </row>
-    <row r="155" spans="1:11">
+      <c r="L154">
+        <v>3.0231887017841599E-2</v>
+      </c>
+      <c r="M154">
+        <v>7.7555969253345902E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -6848,8 +7778,14 @@
       <c r="K155">
         <v>3.5675173059498901E-3</v>
       </c>
-    </row>
-    <row r="156" spans="1:11">
+      <c r="L155">
+        <v>3.7331858297558397E-2</v>
+      </c>
+      <c r="M155">
+        <v>1.19058825252348E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13">
       <c r="A156" t="s">
         <v>175</v>
       </c>
@@ -6886,8 +7822,14 @@
       <c r="K156">
         <v>3.1892894715110998E-3</v>
       </c>
-    </row>
-    <row r="157" spans="1:11">
+      <c r="L156">
+        <v>3.2369837663803497E-2</v>
+      </c>
+      <c r="M156">
+        <v>1.00800702361761E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13">
       <c r="A157" t="s">
         <v>172</v>
       </c>
@@ -6924,8 +7866,14 @@
       <c r="K157">
         <v>6.1893499915593904E-3</v>
       </c>
-    </row>
-    <row r="158" spans="1:11">
+      <c r="L157">
+        <v>5.12765418952668E-2</v>
+      </c>
+      <c r="M157">
+        <v>1.9760212494082201E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13">
       <c r="A158" t="s">
         <v>171</v>
       </c>
@@ -6962,8 +7910,14 @@
       <c r="K158">
         <v>2.7894865915564998E-3</v>
       </c>
-    </row>
-    <row r="159" spans="1:11">
+      <c r="L158">
+        <v>3.3005921012850097E-2</v>
+      </c>
+      <c r="M158">
+        <v>9.2533348505823496E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13">
       <c r="A159" t="s">
         <v>170</v>
       </c>
@@ -7000,8 +7954,14 @@
       <c r="K159">
         <v>4.53943894545711E-3</v>
       </c>
-    </row>
-    <row r="160" spans="1:11">
+      <c r="L159">
+        <v>3.9464306774498498E-2</v>
+      </c>
+      <c r="M159">
+        <v>1.4411892410494599E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13">
       <c r="A160" t="s">
         <v>168</v>
       </c>
@@ -7038,8 +7998,14 @@
       <c r="K160">
         <v>5.3804504207225004E-3</v>
       </c>
-    </row>
-    <row r="161" spans="1:11">
+      <c r="L160">
+        <v>4.4232529161969701E-2</v>
+      </c>
+      <c r="M160">
+        <v>1.6398058230224499E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13">
       <c r="A161" t="s">
         <v>169</v>
       </c>
@@ -7076,8 +8042,14 @@
       <c r="K161">
         <v>3.06685550557161E-3</v>
       </c>
-    </row>
-    <row r="162" spans="1:11">
+      <c r="L161">
+        <v>3.2804327992051498E-2</v>
+      </c>
+      <c r="M161">
+        <v>9.5259455638531595E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13">
       <c r="A162" t="s">
         <v>165</v>
       </c>
@@ -7114,8 +8086,14 @@
       <c r="K162">
         <v>4.18696041473439E-3</v>
       </c>
-    </row>
-    <row r="163" spans="1:11">
+      <c r="L162">
+        <v>4.1121587248154401E-2</v>
+      </c>
+      <c r="M162">
+        <v>1.3596225162397699E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13">
       <c r="A163" t="s">
         <v>166</v>
       </c>
@@ -7152,8 +8130,14 @@
       <c r="K163">
         <v>3.4506554486583001E-3</v>
       </c>
-    </row>
-    <row r="164" spans="1:11">
+      <c r="L163">
+        <v>3.5292451126234699E-2</v>
+      </c>
+      <c r="M163">
+        <v>1.13514623631013E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13">
       <c r="A164" t="s">
         <v>164</v>
       </c>
@@ -7190,8 +8174,14 @@
       <c r="K164">
         <v>3.9337602879716098E-3</v>
       </c>
-    </row>
-    <row r="165" spans="1:11">
+      <c r="L164">
+        <v>3.5317916499603599E-2</v>
+      </c>
+      <c r="M164">
+        <v>1.1711558875188099E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13">
       <c r="A165" t="s">
         <v>144</v>
       </c>
@@ -7228,8 +8218,14 @@
       <c r="K165">
         <v>4.3741945390988798E-3</v>
       </c>
-    </row>
-    <row r="166" spans="1:11">
+      <c r="L165">
+        <v>3.8406685823549801E-2</v>
+      </c>
+      <c r="M165">
+        <v>1.3283871923889501E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13">
       <c r="A166" t="s">
         <v>142</v>
       </c>
@@ -7266,8 +8262,14 @@
       <c r="K166">
         <v>3.71699389882781E-3</v>
       </c>
-    </row>
-    <row r="167" spans="1:11">
+      <c r="L166">
+        <v>3.2982127376997197E-2</v>
+      </c>
+      <c r="M166">
+        <v>1.20324401670524E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13">
       <c r="A167" t="s">
         <v>143</v>
       </c>
@@ -7304,8 +8306,14 @@
       <c r="K167">
         <v>1.6525406154387801E-3</v>
       </c>
-    </row>
-    <row r="168" spans="1:11">
+      <c r="L167">
+        <v>2.80258454026991E-2</v>
+      </c>
+      <c r="M167">
+        <v>6.7335099041055798E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13">
       <c r="A168" t="s">
         <v>146</v>
       </c>
@@ -7342,8 +8350,14 @@
       <c r="K168">
         <v>5.1899015621618503E-3</v>
       </c>
-    </row>
-    <row r="169" spans="1:11">
+      <c r="L168">
+        <v>4.0735096220979303E-2</v>
+      </c>
+      <c r="M168">
+        <v>1.31857154386408E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -7380,8 +8394,14 @@
       <c r="K169">
         <v>2.62570822674243E-3</v>
       </c>
-    </row>
-    <row r="170" spans="1:11">
+      <c r="L169">
+        <v>3.8936051032613099E-2</v>
+      </c>
+      <c r="M169">
+        <v>8.4327036613489198E-3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13">
       <c r="A170" t="s">
         <v>8</v>
       </c>
@@ -7418,8 +8438,14 @@
       <c r="K170">
         <v>2.6413255777415099E-3</v>
       </c>
-    </row>
-    <row r="171" spans="1:11">
+      <c r="L170">
+        <v>3.9491596532109097E-2</v>
+      </c>
+      <c r="M170">
+        <v>8.8349023173879392E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -7456,8 +8482,14 @@
       <c r="K171">
         <v>2.1584915418803698E-3</v>
       </c>
-    </row>
-    <row r="172" spans="1:11">
+      <c r="L171">
+        <v>3.2680618392519699E-2</v>
+      </c>
+      <c r="M171">
+        <v>6.1817277984886404E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13">
       <c r="A172" t="s">
         <v>10</v>
       </c>
@@ -7494,8 +8526,14 @@
       <c r="K172">
         <v>1.66276071575348E-3</v>
       </c>
-    </row>
-    <row r="173" spans="1:11">
+      <c r="L172">
+        <v>3.2309973472867799E-2</v>
+      </c>
+      <c r="M172">
+        <v>6.1323703861595504E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13">
       <c r="A173" t="s">
         <v>6</v>
       </c>
@@ -7532,8 +8570,14 @@
       <c r="K173">
         <v>2.7427745048437999E-3</v>
       </c>
-    </row>
-    <row r="174" spans="1:11">
+      <c r="L173">
+        <v>3.8997539913207202E-2</v>
+      </c>
+      <c r="M173">
+        <v>8.8719468181259198E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -7570,8 +8614,14 @@
       <c r="K174">
         <v>2.3869923648715198E-3</v>
       </c>
-    </row>
-    <row r="175" spans="1:11">
+      <c r="L174">
+        <v>3.8886410481556402E-2</v>
+      </c>
+      <c r="M174">
+        <v>9.4091990213327498E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13">
       <c r="A175" t="s">
         <v>5</v>
       </c>
@@ -7608,8 +8658,14 @@
       <c r="K175">
         <v>3.1622220039792398E-3</v>
       </c>
-    </row>
-    <row r="176" spans="1:11">
+      <c r="L175">
+        <v>3.6753164063223001E-2</v>
+      </c>
+      <c r="M175">
+        <v>9.2628101843995492E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13">
       <c r="A176" t="s">
         <v>4</v>
       </c>
@@ -7646,8 +8702,14 @@
       <c r="K176">
         <v>2.4209048773299398E-3</v>
       </c>
-    </row>
-    <row r="177" spans="1:11">
+      <c r="L176">
+        <v>3.8846271252384601E-2</v>
+      </c>
+      <c r="M176">
+        <v>9.2322860145774201E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13">
       <c r="A177" t="s">
         <v>21</v>
       </c>
@@ -7684,8 +8746,14 @@
       <c r="K177">
         <v>1.5521375614600901E-3</v>
       </c>
-    </row>
-    <row r="178" spans="1:11">
+      <c r="L177">
+        <v>2.9775079237966601E-2</v>
+      </c>
+      <c r="M177">
+        <v>5.7477622862456799E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13">
       <c r="A178" t="s">
         <v>27</v>
       </c>
@@ -7722,8 +8790,14 @@
       <c r="K178">
         <v>2.3727296215051599E-3</v>
       </c>
-    </row>
-    <row r="179" spans="1:11">
+      <c r="L178">
+        <v>4.2119029169070801E-2</v>
+      </c>
+      <c r="M178">
+        <v>1.39919263526817E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13">
       <c r="A179" t="s">
         <v>25</v>
       </c>
@@ -7760,8 +8834,14 @@
       <c r="K179">
         <v>1.6359213454685999E-3</v>
       </c>
-    </row>
-    <row r="180" spans="1:11">
+      <c r="L179">
+        <v>2.8806487064957701E-2</v>
+      </c>
+      <c r="M179">
+        <v>5.4215437067842102E-3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13">
       <c r="A180" t="s">
         <v>24</v>
       </c>
@@ -7798,8 +8878,14 @@
       <c r="K180">
         <v>2.1219737227122499E-3</v>
       </c>
-    </row>
-    <row r="181" spans="1:11">
+      <c r="L180">
+        <v>4.0810800594331502E-2</v>
+      </c>
+      <c r="M180">
+        <v>1.2507861200772101E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13">
       <c r="A181" t="s">
         <v>1</v>
       </c>
@@ -7835,6 +8921,12 @@
       </c>
       <c r="K181">
         <v>2.54443819722904E-3</v>
+      </c>
+      <c r="L181">
+        <v>3.6420763067647403E-2</v>
+      </c>
+      <c r="M181">
+        <v>7.4310540377019096E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>